<commit_message>
more hw 3 stuff
</commit_message>
<xml_diff>
--- a/Interpolator.xlsx
+++ b/Interpolator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vloom\Documents\Masters\Spring 2023\MAE640\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Veronica\Documents\MAE640\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF7D283-E266-4003-8A3F-8637641255EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFDAE81-1645-4145-BEC6-B5233C154560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7110" yWindow="3350" windowWidth="19200" windowHeight="6540" xr2:uid="{44436561-2CEC-46D3-8BCD-E22F02F1E11E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{44436561-2CEC-46D3-8BCD-E22F02F1E11E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -446,21 +446,21 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -474,22 +474,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>9</v>
+        <v>-29.628599999999999</v>
       </c>
       <c r="B7">
-        <v>1.67883</v>
+        <v>5163.7</v>
       </c>
       <c r="D7">
-        <v>9.84</v>
+        <v>0</v>
       </c>
       <c r="F7">
         <f>((B9-B7)/(A9-A7))*(D7-A7)+B7</f>
-        <v>1.6874651999999999</v>
+        <v>5163.9956242942881</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
@@ -497,12 +497,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>10</v>
+        <v>30.505700000000001</v>
       </c>
       <c r="B9">
-        <v>1.6891099999999999</v>
+        <v>5164.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>